<commit_message>
Adds additional probes, and Excel file with Instruction breakout
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6480" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="60">
   <si>
     <t>ALU</t>
   </si>
@@ -1615,7 +1615,7 @@
   <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1891,14 +1891,12 @@
       <c r="G13" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="22" t="s">
-        <v>56</v>
-      </c>
+      <c r="H13" s="22"/>
       <c r="I13" s="22"/>
       <c r="J13" s="21"/>
       <c r="K13" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>3 4</v>
+        <v>3</v>
       </c>
       <c r="L13" s="21"/>
     </row>
@@ -2084,9 +2082,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N21"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4012,8 +4010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Before changing the instruction register order
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6480" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="76">
   <si>
     <t>ALU</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>B=Dest Reg</t>
+  </si>
+  <si>
+    <t>Decode</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
@@ -2777,7 +2780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AG21"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
@@ -3310,8 +3313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AG21"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3420,7 +3423,9 @@
         <v>14</v>
       </c>
       <c r="D2" s="35"/>
-      <c r="E2" s="26"/>
+      <c r="E2" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
@@ -3430,7 +3435,7 @@
       <c r="L2" s="27"/>
       <c r="N2" t="str">
         <f>TRIM(_xlfn.CONCAT(IF(ISBLANK(D2),"",$D$1), " ", IF(ISBLANK(E2),"",$E$1), " ", IF(ISBLANK(F2),"",$F$1), " ", IF(ISBLANK(G2),"",$G$1), " ", IF(ISBLANK(H2),"",$H$1), " ", IF(ISBLANK(I2),"",$I$1), " ", IF(ISBLANK(J2),"",$J$1), " ", IF(ISBLANK(K2),"",$K$1), " ", IF(ISBLANK(L2),"",$L$1)))</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.25">
@@ -3438,7 +3443,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="23"/>
@@ -3458,9 +3463,7 @@
       <c r="B4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>16</v>
-      </c>
+      <c r="C4" s="30"/>
       <c r="D4" s="36"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
@@ -3479,9 +3482,7 @@
       <c r="B5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>17</v>
-      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="36"/>
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
@@ -3500,9 +3501,7 @@
       <c r="B6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>18</v>
-      </c>
+      <c r="C6" s="30"/>
       <c r="D6" s="36"/>
       <c r="E6" s="23"/>
       <c r="F6" s="23"/>
@@ -3521,9 +3520,7 @@
       <c r="B7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>23</v>
-      </c>
+      <c r="C7" s="30"/>
       <c r="D7" s="36"/>
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
@@ -3545,7 +3542,9 @@
       <c r="C8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
@@ -3556,7 +3555,7 @@
       <c r="L8" s="27"/>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3652,7 +3651,9 @@
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
+      <c r="F13" s="26" t="s">
+        <v>56</v>
+      </c>
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
       <c r="I13" s="26"/>
@@ -3661,7 +3662,7 @@
       <c r="L13" s="27"/>
       <c r="N13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.25">
@@ -3671,7 +3672,9 @@
       <c r="C14" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="36" t="s">
+        <v>56</v>
+      </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
@@ -3682,7 +3685,7 @@
       <c r="L14" s="28"/>
       <c r="N14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:33" x14ac:dyDescent="0.25">
@@ -3693,7 +3696,9 @@
         <v>39</v>
       </c>
       <c r="D15" s="36"/>
-      <c r="E15" s="23"/>
+      <c r="E15" s="23" t="s">
+        <v>56</v>
+      </c>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
@@ -3703,7 +3708,7 @@
       <c r="L15" s="28"/>
       <c r="N15" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Program document matches program
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6480" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6480" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="CONST-TO-REG" sheetId="6" r:id="rId6"/>
     <sheet name="REG-2-MEM" sheetId="9" r:id="rId7"/>
     <sheet name="REG-2-REG" sheetId="10" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="132">
   <si>
     <t>ALU</t>
   </si>
@@ -295,6 +297,138 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>SHIFT</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>Llimit</t>
+  </si>
+  <si>
+    <t>Hlimit</t>
+  </si>
+  <si>
+    <t>R2R(R0, R4)</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>LowLimit</t>
+  </si>
+  <si>
+    <t>HighLimit</t>
+  </si>
+  <si>
+    <t>Tmp</t>
+  </si>
+  <si>
+    <t>R2R(R0, R5)</t>
+  </si>
+  <si>
+    <t>R2R(R5, R0)</t>
+  </si>
+  <si>
+    <t>C2R(R1, 0)</t>
+  </si>
+  <si>
+    <t>C2R(R2, 0)</t>
+  </si>
+  <si>
+    <t>C2R(R3, 10)</t>
+  </si>
+  <si>
+    <t>While(true)</t>
+  </si>
+  <si>
+    <t>while(true)</t>
+  </si>
+  <si>
+    <t>innerWhile</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>C2R(R6, 1)</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>Count++</t>
+  </si>
+  <si>
+    <t>JumpToCount++</t>
+  </si>
+  <si>
+    <t>while(count &lt; 10)</t>
+  </si>
+  <si>
+    <t>JumpTo While(true)</t>
+  </si>
+  <si>
+    <t>while(count &gt; 0)</t>
+  </si>
+  <si>
+    <t>R2R(R4, R0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD(R1, R6, R1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB(R1, R6, R1) </t>
+  </si>
+  <si>
+    <t>Count--</t>
+  </si>
+  <si>
+    <t>JumpToCount--</t>
+  </si>
+  <si>
+    <t>Halt</t>
+  </si>
+  <si>
+    <t>SUB(R1, R3, R7)</t>
+  </si>
+  <si>
+    <t>SUB(R1, R2, R7)</t>
+  </si>
+  <si>
+    <t>Do while</t>
   </si>
 </sst>
 </file>
@@ -332,7 +466,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,8 +509,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -756,11 +896,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -977,6 +1228,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -986,6 +1246,149 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1305,7 +1708,7 @@
   <dimension ref="A2:AA21"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B2" sqref="B2:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,11 +2143,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V8" s="75" t="s">
+      <c r="V8" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="W8" s="75"/>
-      <c r="X8" s="75"/>
+      <c r="W8" s="78"/>
+      <c r="X8" s="78"/>
       <c r="Z8" s="14" t="s">
         <v>28</v>
       </c>
@@ -1860,6 +2263,308 @@
   <mergeCells count="1">
     <mergeCell ref="V8:X8"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.125" customWidth="1"/>
+    <col min="2" max="8" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="75"/>
+      <c r="B1" s="75">
+        <v>6</v>
+      </c>
+      <c r="C1" s="75">
+        <v>5</v>
+      </c>
+      <c r="D1" s="75">
+        <v>4</v>
+      </c>
+      <c r="E1" s="75">
+        <v>3</v>
+      </c>
+      <c r="F1" s="75">
+        <v>2</v>
+      </c>
+      <c r="G1" s="75">
+        <v>1</v>
+      </c>
+      <c r="H1" s="75">
+        <v>0</v>
+      </c>
+      <c r="I1" s="75"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="75">
+        <v>0</v>
+      </c>
+      <c r="B2" s="126">
+        <v>1</v>
+      </c>
+      <c r="C2" s="127">
+        <v>1</v>
+      </c>
+      <c r="D2" s="127">
+        <v>1</v>
+      </c>
+      <c r="E2" s="127">
+        <v>1</v>
+      </c>
+      <c r="F2" s="127">
+        <v>1</v>
+      </c>
+      <c r="G2" s="127">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="75"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="75">
+        <v>1</v>
+      </c>
+      <c r="B3" s="128">
+        <v>1</v>
+      </c>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129">
+        <v>1</v>
+      </c>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="75"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="75">
+        <v>2</v>
+      </c>
+      <c r="B4" s="128"/>
+      <c r="C4" s="129">
+        <v>1</v>
+      </c>
+      <c r="D4" s="129">
+        <v>1</v>
+      </c>
+      <c r="E4" s="129">
+        <v>1</v>
+      </c>
+      <c r="F4" s="129">
+        <v>1</v>
+      </c>
+      <c r="G4" s="129"/>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="75"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="75">
+        <v>3</v>
+      </c>
+      <c r="B5" s="128">
+        <v>1</v>
+      </c>
+      <c r="C5" s="129">
+        <v>1</v>
+      </c>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129">
+        <v>1</v>
+      </c>
+      <c r="F5" s="129">
+        <v>1</v>
+      </c>
+      <c r="G5" s="129"/>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="75"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
+        <v>4</v>
+      </c>
+      <c r="B6" s="128">
+        <v>1</v>
+      </c>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129">
+        <v>1</v>
+      </c>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="75"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="75">
+        <v>5</v>
+      </c>
+      <c r="B7" s="128">
+        <v>1</v>
+      </c>
+      <c r="C7" s="129">
+        <v>1</v>
+      </c>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129">
+        <v>1</v>
+      </c>
+      <c r="G7" s="129">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="75"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="75">
+        <v>6</v>
+      </c>
+      <c r="B8" s="128">
+        <v>1</v>
+      </c>
+      <c r="C8" s="129">
+        <v>1</v>
+      </c>
+      <c r="D8" s="129">
+        <v>1</v>
+      </c>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129">
+        <v>1</v>
+      </c>
+      <c r="G8" s="129">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="75"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="75">
+        <v>7</v>
+      </c>
+      <c r="B9" s="128">
+        <v>1</v>
+      </c>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129">
+        <v>1</v>
+      </c>
+      <c r="F9" s="129">
+        <v>1</v>
+      </c>
+      <c r="G9" s="129"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="75"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="75">
+        <v>8</v>
+      </c>
+      <c r="B10" s="128">
+        <v>1</v>
+      </c>
+      <c r="C10" s="129">
+        <v>1</v>
+      </c>
+      <c r="D10" s="129">
+        <v>1</v>
+      </c>
+      <c r="E10" s="129">
+        <v>1</v>
+      </c>
+      <c r="F10" s="129">
+        <v>1</v>
+      </c>
+      <c r="G10" s="129">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="75"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="75">
+        <v>9</v>
+      </c>
+      <c r="B11" s="130">
+        <v>1</v>
+      </c>
+      <c r="C11" s="131"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="131">
+        <v>1</v>
+      </c>
+      <c r="F11" s="131">
+        <v>1</v>
+      </c>
+      <c r="G11" s="131">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1</v>
+      </c>
+      <c r="I11" s="75"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="75"/>
+      <c r="B12" s="75">
+        <f t="shared" ref="B12" si="0">SUM(B2:B11)</f>
+        <v>9</v>
+      </c>
+      <c r="C12" s="75">
+        <f>SUM(C2:C11)</f>
+        <v>6</v>
+      </c>
+      <c r="D12" s="75">
+        <f>SUM(D2:D11)</f>
+        <v>4</v>
+      </c>
+      <c r="E12" s="75">
+        <f>SUM(E2:E11)</f>
+        <v>8</v>
+      </c>
+      <c r="F12" s="75">
+        <f>SUM(F2:F11)</f>
+        <v>8</v>
+      </c>
+      <c r="G12" s="75">
+        <f>SUM(G2:G11)</f>
+        <v>6</v>
+      </c>
+      <c r="H12" s="75">
+        <f>SUM(H2:H11)</f>
+        <v>7</v>
+      </c>
+      <c r="I12" s="75"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1905,10 +2610,10 @@
       <c r="C9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="76" t="s">
+      <c r="D9" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="76"/>
+      <c r="E9" s="79"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -1945,10 +2650,10 @@
       <c r="C13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="76" t="s">
+      <c r="D13" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="76"/>
+      <c r="E13" s="79"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -1957,10 +2662,10 @@
       <c r="C14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="76" t="s">
+      <c r="D14" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="76"/>
+      <c r="E14" s="79"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -3058,9 +3763,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA16"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3173,16 +3878,16 @@
         <f>TRIM(_xlfn.CONCAT(IF(ISBLANK(D2),"",$D$1), " ", IF(ISBLANK(E2),"",$E$1), " ", IF(ISBLANK(F2),"",$F$1), " ", IF(ISBLANK(G2),"",$G$1), " ", IF(ISBLANK(H2),"",$H$1), " ", IF(ISBLANK(I2),"",$I$1), " ", IF(ISBLANK(J2),"",$J$1), " ", IF(ISBLANK(K2),"",$K$1), " ", IF(ISBLANK(L2),"",$L$1)))</f>
         <v>0 2</v>
       </c>
-      <c r="Q2" s="77" t="s">
+      <c r="Q2" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="78" t="s">
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
@@ -4137,16 +4842,16 @@
         <f>TRIM(_xlfn.CONCAT(IF(ISBLANK(D2),"",$D$1), " ", IF(ISBLANK(E2),"",$E$1), " ", IF(ISBLANK(F2),"",$F$1), " ", IF(ISBLANK(G2),"",$G$1), " ", IF(ISBLANK(H2),"",$H$1), " ", IF(ISBLANK(I2),"",$I$1), " ", IF(ISBLANK(J2),"",$J$1), " ", IF(ISBLANK(K2),"",$K$1), " ", IF(ISBLANK(L2),"",$L$1)))</f>
         <v>0 2</v>
       </c>
-      <c r="Q2" s="77" t="s">
+      <c r="Q2" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="78" t="s">
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
@@ -4511,9 +5216,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4626,16 +5331,16 @@
         <f>TRIM(_xlfn.CONCAT(IF(ISBLANK(D2),"",$D$1), " ", IF(ISBLANK(E2),"",$E$1), " ", IF(ISBLANK(F2),"",$F$1), " ", IF(ISBLANK(G2),"",$G$1), " ", IF(ISBLANK(H2),"",$H$1), " ", IF(ISBLANK(I2),"",$I$1), " ", IF(ISBLANK(J2),"",$J$1), " ", IF(ISBLANK(K2),"",$K$1), " ", IF(ISBLANK(L2),"",$L$1)))</f>
         <v>1 3</v>
       </c>
-      <c r="Q2" s="77" t="s">
+      <c r="Q2" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="77"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="78" t="s">
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
@@ -5010,4 +5715,1449 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.125" customWidth="1"/>
+    <col min="2" max="2" width="14.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="19" width="3.5" customWidth="1"/>
+    <col min="20" max="20" width="6.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C1" s="2"/>
+      <c r="D1" s="75">
+        <v>15</v>
+      </c>
+      <c r="E1" s="75">
+        <v>14</v>
+      </c>
+      <c r="F1" s="75">
+        <v>13</v>
+      </c>
+      <c r="G1" s="75">
+        <v>12</v>
+      </c>
+      <c r="H1" s="75">
+        <v>11</v>
+      </c>
+      <c r="I1" s="75">
+        <v>10</v>
+      </c>
+      <c r="J1" s="75">
+        <v>9</v>
+      </c>
+      <c r="K1" s="75">
+        <v>8</v>
+      </c>
+      <c r="L1" s="75">
+        <v>7</v>
+      </c>
+      <c r="M1" s="75">
+        <v>6</v>
+      </c>
+      <c r="N1" s="75">
+        <v>5</v>
+      </c>
+      <c r="O1" s="75">
+        <v>4</v>
+      </c>
+      <c r="P1" s="75">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="75">
+        <v>2</v>
+      </c>
+      <c r="R1" s="75">
+        <v>1</v>
+      </c>
+      <c r="S1" s="75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="50">
+        <v>1</v>
+      </c>
+      <c r="E2" s="45">
+        <v>0</v>
+      </c>
+      <c r="F2" s="45">
+        <v>0</v>
+      </c>
+      <c r="G2" s="45">
+        <v>1</v>
+      </c>
+      <c r="H2" s="45">
+        <v>1</v>
+      </c>
+      <c r="I2" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="44">
+        <v>0</v>
+      </c>
+      <c r="S2" s="44">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>95</v>
+      </c>
+      <c r="V2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="50">
+        <v>1</v>
+      </c>
+      <c r="E3" s="45">
+        <v>0</v>
+      </c>
+      <c r="F3" s="45">
+        <v>1</v>
+      </c>
+      <c r="G3" s="45">
+        <v>1</v>
+      </c>
+      <c r="H3" s="45">
+        <v>1</v>
+      </c>
+      <c r="I3" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="44">
+        <v>0</v>
+      </c>
+      <c r="S3" s="44">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>88</v>
+      </c>
+      <c r="V3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="50">
+        <v>1</v>
+      </c>
+      <c r="E4" s="45">
+        <v>0</v>
+      </c>
+      <c r="F4" s="45">
+        <v>0</v>
+      </c>
+      <c r="G4" s="45">
+        <v>0</v>
+      </c>
+      <c r="H4" s="45">
+        <v>0</v>
+      </c>
+      <c r="I4" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="44">
+        <v>0</v>
+      </c>
+      <c r="S4" s="44">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>96</v>
+      </c>
+      <c r="V4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="50">
+        <v>0</v>
+      </c>
+      <c r="E5" s="44">
+        <v>0</v>
+      </c>
+      <c r="F5" s="44">
+        <v>0</v>
+      </c>
+      <c r="G5" s="51">
+        <v>0</v>
+      </c>
+      <c r="H5" s="51">
+        <v>0</v>
+      </c>
+      <c r="I5" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="44">
+        <v>0</v>
+      </c>
+      <c r="P5" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="44">
+        <v>0</v>
+      </c>
+      <c r="R5" s="44">
+        <v>0</v>
+      </c>
+      <c r="S5" s="44">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>97</v>
+      </c>
+      <c r="V5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="50">
+        <v>0</v>
+      </c>
+      <c r="E6" s="44">
+        <v>0</v>
+      </c>
+      <c r="F6" s="44">
+        <v>0</v>
+      </c>
+      <c r="G6" s="51">
+        <v>0</v>
+      </c>
+      <c r="H6" s="51">
+        <v>1</v>
+      </c>
+      <c r="I6" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" t="s">
+        <v>98</v>
+      </c>
+      <c r="V6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="50">
+        <v>0</v>
+      </c>
+      <c r="E7" s="44">
+        <v>0</v>
+      </c>
+      <c r="F7" s="44">
+        <v>0</v>
+      </c>
+      <c r="G7" s="51">
+        <v>1</v>
+      </c>
+      <c r="H7" s="51">
+        <v>0</v>
+      </c>
+      <c r="I7" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="44">
+        <v>0</v>
+      </c>
+      <c r="P7" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="44">
+        <v>0</v>
+      </c>
+      <c r="R7" s="44">
+        <v>0</v>
+      </c>
+      <c r="S7" s="44">
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
+        <v>99</v>
+      </c>
+      <c r="V7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="50">
+        <v>0</v>
+      </c>
+      <c r="E8" s="44">
+        <v>0</v>
+      </c>
+      <c r="F8" s="44">
+        <v>0</v>
+      </c>
+      <c r="G8" s="51">
+        <v>1</v>
+      </c>
+      <c r="H8" s="51">
+        <v>1</v>
+      </c>
+      <c r="I8" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="44">
+        <v>0</v>
+      </c>
+      <c r="S8" s="44">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
+        <v>100</v>
+      </c>
+      <c r="V8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U9" t="s">
+        <v>101</v>
+      </c>
+      <c r="V9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="50">
+        <v>0</v>
+      </c>
+      <c r="E12" s="44">
+        <v>0</v>
+      </c>
+      <c r="F12" s="44">
+        <v>0</v>
+      </c>
+      <c r="G12" s="51">
+        <v>0</v>
+      </c>
+      <c r="H12" s="51">
+        <v>1</v>
+      </c>
+      <c r="I12" s="76">
+        <v>0</v>
+      </c>
+      <c r="J12" s="76">
+        <v>0</v>
+      </c>
+      <c r="K12" s="76">
+        <v>1</v>
+      </c>
+      <c r="L12" s="49">
+        <v>0</v>
+      </c>
+      <c r="M12" s="49">
+        <v>0</v>
+      </c>
+      <c r="N12" s="49">
+        <v>0</v>
+      </c>
+      <c r="O12" s="49">
+        <v>0</v>
+      </c>
+      <c r="P12" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="49">
+        <v>0</v>
+      </c>
+      <c r="R12" s="49">
+        <v>0</v>
+      </c>
+      <c r="S12" s="49">
+        <v>0</v>
+      </c>
+      <c r="T12" t="str">
+        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(D12:K12), 2),BIN2HEX(_xlfn.CONCAT(L12:S12), 2))</f>
+        <v>0900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="50">
+        <v>0</v>
+      </c>
+      <c r="E13" s="44">
+        <v>0</v>
+      </c>
+      <c r="F13" s="44">
+        <v>0</v>
+      </c>
+      <c r="G13" s="51">
+        <v>0</v>
+      </c>
+      <c r="H13" s="51">
+        <v>1</v>
+      </c>
+      <c r="I13" s="76">
+        <v>0</v>
+      </c>
+      <c r="J13" s="76">
+        <v>1</v>
+      </c>
+      <c r="K13" s="76">
+        <v>0</v>
+      </c>
+      <c r="L13" s="49">
+        <v>0</v>
+      </c>
+      <c r="M13" s="49">
+        <v>0</v>
+      </c>
+      <c r="N13" s="49">
+        <v>0</v>
+      </c>
+      <c r="O13" s="49">
+        <v>0</v>
+      </c>
+      <c r="P13" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="49">
+        <v>0</v>
+      </c>
+      <c r="R13" s="49">
+        <v>0</v>
+      </c>
+      <c r="S13" s="49">
+        <v>0</v>
+      </c>
+      <c r="T13" t="str">
+        <f t="shared" ref="T13:T26" si="0">_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(D13:K13), 2),BIN2HEX(_xlfn.CONCAT(L13:S13), 2))</f>
+        <v>0A00</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="50">
+        <v>0</v>
+      </c>
+      <c r="E14" s="44">
+        <v>0</v>
+      </c>
+      <c r="F14" s="44">
+        <v>0</v>
+      </c>
+      <c r="G14" s="51">
+        <v>0</v>
+      </c>
+      <c r="H14" s="51">
+        <v>1</v>
+      </c>
+      <c r="I14" s="76">
+        <v>0</v>
+      </c>
+      <c r="J14" s="76">
+        <v>1</v>
+      </c>
+      <c r="K14" s="76">
+        <v>1</v>
+      </c>
+      <c r="L14" s="49">
+        <v>0</v>
+      </c>
+      <c r="M14" s="49">
+        <v>0</v>
+      </c>
+      <c r="N14" s="49">
+        <v>0</v>
+      </c>
+      <c r="O14" s="49">
+        <v>0</v>
+      </c>
+      <c r="P14" s="49">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="49">
+        <v>0</v>
+      </c>
+      <c r="R14" s="49">
+        <v>1</v>
+      </c>
+      <c r="S14" s="49">
+        <v>0</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" si="0"/>
+        <v>0B0A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="50">
+        <v>0</v>
+      </c>
+      <c r="E15" s="44">
+        <v>0</v>
+      </c>
+      <c r="F15" s="44">
+        <v>0</v>
+      </c>
+      <c r="G15" s="51">
+        <v>0</v>
+      </c>
+      <c r="H15" s="51">
+        <v>1</v>
+      </c>
+      <c r="I15" s="76">
+        <v>1</v>
+      </c>
+      <c r="J15" s="76">
+        <v>1</v>
+      </c>
+      <c r="K15" s="76">
+        <v>0</v>
+      </c>
+      <c r="L15" s="49">
+        <v>0</v>
+      </c>
+      <c r="M15" s="49">
+        <v>0</v>
+      </c>
+      <c r="N15" s="49">
+        <v>0</v>
+      </c>
+      <c r="O15" s="49">
+        <v>0</v>
+      </c>
+      <c r="P15" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="49">
+        <v>0</v>
+      </c>
+      <c r="R15" s="49">
+        <v>0</v>
+      </c>
+      <c r="S15" s="49">
+        <v>1</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="0"/>
+        <v>0E01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="83" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="84">
+        <v>0</v>
+      </c>
+      <c r="E16" s="85">
+        <v>0</v>
+      </c>
+      <c r="F16" s="85">
+        <v>0</v>
+      </c>
+      <c r="G16" s="86">
+        <v>1</v>
+      </c>
+      <c r="H16" s="86">
+        <v>1</v>
+      </c>
+      <c r="I16" s="87">
+        <v>0</v>
+      </c>
+      <c r="J16" s="87">
+        <v>0</v>
+      </c>
+      <c r="K16" s="87">
+        <v>0</v>
+      </c>
+      <c r="L16" s="122">
+        <v>1</v>
+      </c>
+      <c r="M16" s="122">
+        <v>0</v>
+      </c>
+      <c r="N16" s="122">
+        <v>0</v>
+      </c>
+      <c r="O16" s="123">
+        <v>1</v>
+      </c>
+      <c r="P16" s="123">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="123">
+        <v>1</v>
+      </c>
+      <c r="R16" s="85">
+        <v>0</v>
+      </c>
+      <c r="S16" s="124">
+        <v>0</v>
+      </c>
+      <c r="T16" t="str">
+        <f t="shared" si="0"/>
+        <v>189C</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" s="117" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="106" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="107">
+        <v>0</v>
+      </c>
+      <c r="E17" s="108">
+        <v>0</v>
+      </c>
+      <c r="F17" s="108">
+        <v>0</v>
+      </c>
+      <c r="G17" s="109">
+        <v>1</v>
+      </c>
+      <c r="H17" s="109">
+        <v>1</v>
+      </c>
+      <c r="I17" s="110">
+        <v>0</v>
+      </c>
+      <c r="J17" s="110">
+        <v>0</v>
+      </c>
+      <c r="K17" s="110">
+        <v>0</v>
+      </c>
+      <c r="L17" s="121">
+        <v>1</v>
+      </c>
+      <c r="M17" s="121">
+        <v>0</v>
+      </c>
+      <c r="N17" s="121">
+        <v>1</v>
+      </c>
+      <c r="O17" s="120">
+        <v>1</v>
+      </c>
+      <c r="P17" s="120">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="120">
+        <v>1</v>
+      </c>
+      <c r="R17" s="108">
+        <v>0</v>
+      </c>
+      <c r="S17" s="125">
+        <v>0</v>
+      </c>
+      <c r="T17" t="str">
+        <f t="shared" si="0"/>
+        <v>18BC</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="89" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" s="90">
+        <v>1</v>
+      </c>
+      <c r="E18" s="91">
+        <v>0</v>
+      </c>
+      <c r="F18" s="91">
+        <v>0</v>
+      </c>
+      <c r="G18" s="91">
+        <v>1</v>
+      </c>
+      <c r="H18" s="91">
+        <v>1</v>
+      </c>
+      <c r="I18" s="92">
+        <v>0</v>
+      </c>
+      <c r="J18" s="92">
+        <v>0</v>
+      </c>
+      <c r="K18" s="92">
+        <v>1</v>
+      </c>
+      <c r="L18" s="93">
+        <v>1</v>
+      </c>
+      <c r="M18" s="93">
+        <v>1</v>
+      </c>
+      <c r="N18" s="93">
+        <v>0</v>
+      </c>
+      <c r="O18" s="94">
+        <v>0</v>
+      </c>
+      <c r="P18" s="94">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="94">
+        <v>1</v>
+      </c>
+      <c r="R18" s="95">
+        <v>0</v>
+      </c>
+      <c r="S18" s="96">
+        <v>0</v>
+      </c>
+      <c r="T18" t="str">
+        <f t="shared" si="0"/>
+        <v>99C4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" s="88" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="89"/>
+      <c r="D19" s="90">
+        <v>1</v>
+      </c>
+      <c r="E19" s="91">
+        <v>0</v>
+      </c>
+      <c r="F19" s="91">
+        <v>1</v>
+      </c>
+      <c r="G19" s="91">
+        <v>1</v>
+      </c>
+      <c r="H19" s="91">
+        <v>1</v>
+      </c>
+      <c r="I19" s="92">
+        <v>0</v>
+      </c>
+      <c r="J19" s="92">
+        <v>1</v>
+      </c>
+      <c r="K19" s="92">
+        <v>1</v>
+      </c>
+      <c r="L19" s="93">
+        <v>0</v>
+      </c>
+      <c r="M19" s="93">
+        <v>0</v>
+      </c>
+      <c r="N19" s="93">
+        <v>1</v>
+      </c>
+      <c r="O19" s="94">
+        <v>1</v>
+      </c>
+      <c r="P19" s="94">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="94">
+        <v>1</v>
+      </c>
+      <c r="R19" s="95">
+        <v>0</v>
+      </c>
+      <c r="S19" s="96">
+        <v>0</v>
+      </c>
+      <c r="T19" t="str">
+        <f t="shared" si="0"/>
+        <v>BB3C</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20" s="118" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="111" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="112">
+        <v>0</v>
+      </c>
+      <c r="E20" s="113">
+        <v>0</v>
+      </c>
+      <c r="F20" s="113">
+        <v>0</v>
+      </c>
+      <c r="G20" s="114">
+        <v>1</v>
+      </c>
+      <c r="H20" s="114">
+        <v>1</v>
+      </c>
+      <c r="I20" s="115">
+        <v>1</v>
+      </c>
+      <c r="J20" s="115">
+        <v>0</v>
+      </c>
+      <c r="K20" s="115">
+        <v>1</v>
+      </c>
+      <c r="L20" s="116">
+        <v>0</v>
+      </c>
+      <c r="M20" s="116">
+        <v>0</v>
+      </c>
+      <c r="N20" s="116">
+        <v>0</v>
+      </c>
+      <c r="O20" s="132">
+        <v>0</v>
+      </c>
+      <c r="P20" s="132">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="132">
+        <v>1</v>
+      </c>
+      <c r="R20" s="113">
+        <v>0</v>
+      </c>
+      <c r="S20" s="119">
+        <v>0</v>
+      </c>
+      <c r="T20" t="str">
+        <f t="shared" si="0"/>
+        <v>1D04</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21" s="117" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="106" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="107">
+        <v>0</v>
+      </c>
+      <c r="E21" s="108">
+        <v>0</v>
+      </c>
+      <c r="F21" s="108">
+        <v>0</v>
+      </c>
+      <c r="G21" s="109">
+        <v>1</v>
+      </c>
+      <c r="H21" s="109">
+        <v>1</v>
+      </c>
+      <c r="I21" s="110">
+        <v>0</v>
+      </c>
+      <c r="J21" s="110">
+        <v>0</v>
+      </c>
+      <c r="K21" s="110">
+        <v>0</v>
+      </c>
+      <c r="L21" s="121">
+        <v>1</v>
+      </c>
+      <c r="M21" s="121">
+        <v>0</v>
+      </c>
+      <c r="N21" s="121">
+        <v>1</v>
+      </c>
+      <c r="O21" s="120">
+        <v>1</v>
+      </c>
+      <c r="P21" s="120">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="120">
+        <v>1</v>
+      </c>
+      <c r="R21" s="108">
+        <v>0</v>
+      </c>
+      <c r="S21" s="125">
+        <v>0</v>
+      </c>
+      <c r="T21" t="str">
+        <f t="shared" si="0"/>
+        <v>18BC</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22" s="88" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="89" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="90">
+        <v>1</v>
+      </c>
+      <c r="E22" s="91">
+        <v>0</v>
+      </c>
+      <c r="F22" s="91">
+        <v>1</v>
+      </c>
+      <c r="G22" s="91">
+        <v>1</v>
+      </c>
+      <c r="H22" s="91">
+        <v>1</v>
+      </c>
+      <c r="I22" s="92">
+        <v>0</v>
+      </c>
+      <c r="J22" s="92">
+        <v>0</v>
+      </c>
+      <c r="K22" s="92">
+        <v>1</v>
+      </c>
+      <c r="L22" s="93">
+        <v>1</v>
+      </c>
+      <c r="M22" s="93">
+        <v>1</v>
+      </c>
+      <c r="N22" s="93">
+        <v>0</v>
+      </c>
+      <c r="O22" s="94">
+        <v>0</v>
+      </c>
+      <c r="P22" s="94">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="94">
+        <v>1</v>
+      </c>
+      <c r="R22" s="95">
+        <v>0</v>
+      </c>
+      <c r="S22" s="96">
+        <v>0</v>
+      </c>
+      <c r="T22" t="str">
+        <f t="shared" si="0"/>
+        <v>B9C4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23" s="88" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="89"/>
+      <c r="D23" s="90">
+        <v>1</v>
+      </c>
+      <c r="E23" s="91">
+        <v>0</v>
+      </c>
+      <c r="F23" s="91">
+        <v>1</v>
+      </c>
+      <c r="G23" s="91">
+        <v>1</v>
+      </c>
+      <c r="H23" s="91">
+        <v>1</v>
+      </c>
+      <c r="I23" s="92">
+        <v>0</v>
+      </c>
+      <c r="J23" s="92">
+        <v>0</v>
+      </c>
+      <c r="K23" s="92">
+        <v>1</v>
+      </c>
+      <c r="L23" s="93">
+        <v>0</v>
+      </c>
+      <c r="M23" s="93">
+        <v>1</v>
+      </c>
+      <c r="N23" s="93">
+        <v>0</v>
+      </c>
+      <c r="O23" s="94">
+        <v>1</v>
+      </c>
+      <c r="P23" s="94">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="94">
+        <v>1</v>
+      </c>
+      <c r="R23" s="95">
+        <v>0</v>
+      </c>
+      <c r="S23" s="96">
+        <v>0</v>
+      </c>
+      <c r="T23" t="str">
+        <f t="shared" si="0"/>
+        <v>B95C</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24" s="118" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="111" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="112">
+        <v>0</v>
+      </c>
+      <c r="E24" s="113">
+        <v>0</v>
+      </c>
+      <c r="F24" s="113">
+        <v>0</v>
+      </c>
+      <c r="G24" s="114">
+        <v>1</v>
+      </c>
+      <c r="H24" s="114">
+        <v>1</v>
+      </c>
+      <c r="I24" s="115">
+        <v>1</v>
+      </c>
+      <c r="J24" s="115">
+        <v>0</v>
+      </c>
+      <c r="K24" s="115">
+        <v>1</v>
+      </c>
+      <c r="L24" s="116">
+        <v>0</v>
+      </c>
+      <c r="M24" s="116">
+        <v>0</v>
+      </c>
+      <c r="N24" s="116">
+        <v>0</v>
+      </c>
+      <c r="O24" s="132">
+        <v>1</v>
+      </c>
+      <c r="P24" s="132">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="132">
+        <v>0</v>
+      </c>
+      <c r="R24" s="113">
+        <v>0</v>
+      </c>
+      <c r="S24" s="119">
+        <v>0</v>
+      </c>
+      <c r="T24" t="str">
+        <f t="shared" si="0"/>
+        <v>1D10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>13</v>
+      </c>
+      <c r="B25" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="C25" s="98" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="99">
+        <v>0</v>
+      </c>
+      <c r="E25" s="100">
+        <v>0</v>
+      </c>
+      <c r="F25" s="100">
+        <v>0</v>
+      </c>
+      <c r="G25" s="101">
+        <v>1</v>
+      </c>
+      <c r="H25" s="101">
+        <v>1</v>
+      </c>
+      <c r="I25" s="102">
+        <v>1</v>
+      </c>
+      <c r="J25" s="102">
+        <v>0</v>
+      </c>
+      <c r="K25" s="102">
+        <v>1</v>
+      </c>
+      <c r="L25" s="103">
+        <v>0</v>
+      </c>
+      <c r="M25" s="103">
+        <v>0</v>
+      </c>
+      <c r="N25" s="103">
+        <v>0</v>
+      </c>
+      <c r="O25" s="104">
+        <v>1</v>
+      </c>
+      <c r="P25" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="104">
+        <v>1</v>
+      </c>
+      <c r="R25" s="100">
+        <v>0</v>
+      </c>
+      <c r="S25" s="105">
+        <v>0</v>
+      </c>
+      <c r="T25" t="str">
+        <f t="shared" si="0"/>
+        <v>1D1C</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed small bug in program and removed debugging outputs
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -1236,6 +1236,149 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1246,149 +1389,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2143,11 +2143,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V8" s="78" t="s">
+      <c r="V8" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="W8" s="78"/>
-      <c r="X8" s="78"/>
+      <c r="W8" s="129"/>
+      <c r="X8" s="129"/>
       <c r="Z8" s="14" t="s">
         <v>28</v>
       </c>
@@ -2310,22 +2310,22 @@
       <c r="A2" s="75">
         <v>0</v>
       </c>
-      <c r="B2" s="126">
-        <v>1</v>
-      </c>
-      <c r="C2" s="127">
-        <v>1</v>
-      </c>
-      <c r="D2" s="127">
-        <v>1</v>
-      </c>
-      <c r="E2" s="127">
-        <v>1</v>
-      </c>
-      <c r="F2" s="127">
-        <v>1</v>
-      </c>
-      <c r="G2" s="127">
+      <c r="B2" s="122">
+        <v>1</v>
+      </c>
+      <c r="C2" s="123">
+        <v>1</v>
+      </c>
+      <c r="D2" s="123">
+        <v>1</v>
+      </c>
+      <c r="E2" s="123">
+        <v>1</v>
+      </c>
+      <c r="F2" s="123">
+        <v>1</v>
+      </c>
+      <c r="G2" s="123">
         <v>1</v>
       </c>
       <c r="H2" s="6"/>
@@ -2335,16 +2335,16 @@
       <c r="A3" s="75">
         <v>1</v>
       </c>
-      <c r="B3" s="128">
-        <v>1</v>
-      </c>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129">
-        <v>1</v>
-      </c>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
+      <c r="B3" s="124">
+        <v>1</v>
+      </c>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125">
+        <v>1</v>
+      </c>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
       <c r="H3" s="4"/>
       <c r="I3" s="75"/>
     </row>
@@ -2352,20 +2352,20 @@
       <c r="A4" s="75">
         <v>2</v>
       </c>
-      <c r="B4" s="128"/>
-      <c r="C4" s="129">
-        <v>1</v>
-      </c>
-      <c r="D4" s="129">
-        <v>1</v>
-      </c>
-      <c r="E4" s="129">
-        <v>1</v>
-      </c>
-      <c r="F4" s="129">
-        <v>1</v>
-      </c>
-      <c r="G4" s="129"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="125">
+        <v>1</v>
+      </c>
+      <c r="D4" s="125">
+        <v>1</v>
+      </c>
+      <c r="E4" s="125">
+        <v>1</v>
+      </c>
+      <c r="F4" s="125">
+        <v>1</v>
+      </c>
+      <c r="G4" s="125"/>
       <c r="H4" s="4">
         <v>1</v>
       </c>
@@ -2375,20 +2375,20 @@
       <c r="A5" s="75">
         <v>3</v>
       </c>
-      <c r="B5" s="128">
-        <v>1</v>
-      </c>
-      <c r="C5" s="129">
-        <v>1</v>
-      </c>
-      <c r="D5" s="129"/>
-      <c r="E5" s="129">
-        <v>1</v>
-      </c>
-      <c r="F5" s="129">
-        <v>1</v>
-      </c>
-      <c r="G5" s="129"/>
+      <c r="B5" s="124">
+        <v>1</v>
+      </c>
+      <c r="C5" s="125">
+        <v>1</v>
+      </c>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125">
+        <v>1</v>
+      </c>
+      <c r="F5" s="125">
+        <v>1</v>
+      </c>
+      <c r="G5" s="125"/>
       <c r="H5" s="4">
         <v>1</v>
       </c>
@@ -2398,16 +2398,16 @@
       <c r="A6" s="75">
         <v>4</v>
       </c>
-      <c r="B6" s="128">
-        <v>1</v>
-      </c>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129">
-        <v>1</v>
-      </c>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129">
+      <c r="B6" s="124">
+        <v>1</v>
+      </c>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125">
+        <v>1</v>
+      </c>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125">
         <v>1</v>
       </c>
       <c r="H6" s="4">
@@ -2419,18 +2419,18 @@
       <c r="A7" s="75">
         <v>5</v>
       </c>
-      <c r="B7" s="128">
-        <v>1</v>
-      </c>
-      <c r="C7" s="129">
-        <v>1</v>
-      </c>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129">
-        <v>1</v>
-      </c>
-      <c r="G7" s="129">
+      <c r="B7" s="124">
+        <v>1</v>
+      </c>
+      <c r="C7" s="125">
+        <v>1</v>
+      </c>
+      <c r="D7" s="125"/>
+      <c r="E7" s="125"/>
+      <c r="F7" s="125">
+        <v>1</v>
+      </c>
+      <c r="G7" s="125">
         <v>1</v>
       </c>
       <c r="H7" s="4">
@@ -2442,20 +2442,20 @@
       <c r="A8" s="75">
         <v>6</v>
       </c>
-      <c r="B8" s="128">
-        <v>1</v>
-      </c>
-      <c r="C8" s="129">
-        <v>1</v>
-      </c>
-      <c r="D8" s="129">
-        <v>1</v>
-      </c>
-      <c r="E8" s="129"/>
-      <c r="F8" s="129">
-        <v>1</v>
-      </c>
-      <c r="G8" s="129">
+      <c r="B8" s="124">
+        <v>1</v>
+      </c>
+      <c r="C8" s="125">
+        <v>1</v>
+      </c>
+      <c r="D8" s="125">
+        <v>1</v>
+      </c>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125">
+        <v>1</v>
+      </c>
+      <c r="G8" s="125">
         <v>1</v>
       </c>
       <c r="H8" s="4">
@@ -2467,18 +2467,18 @@
       <c r="A9" s="75">
         <v>7</v>
       </c>
-      <c r="B9" s="128">
-        <v>1</v>
-      </c>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
-      <c r="E9" s="129">
-        <v>1</v>
-      </c>
-      <c r="F9" s="129">
-        <v>1</v>
-      </c>
-      <c r="G9" s="129"/>
+      <c r="B9" s="124">
+        <v>1</v>
+      </c>
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="125">
+        <v>1</v>
+      </c>
+      <c r="F9" s="125">
+        <v>1</v>
+      </c>
+      <c r="G9" s="125"/>
       <c r="H9" s="4"/>
       <c r="I9" s="75"/>
     </row>
@@ -2486,22 +2486,22 @@
       <c r="A10" s="75">
         <v>8</v>
       </c>
-      <c r="B10" s="128">
-        <v>1</v>
-      </c>
-      <c r="C10" s="129">
-        <v>1</v>
-      </c>
-      <c r="D10" s="129">
-        <v>1</v>
-      </c>
-      <c r="E10" s="129">
-        <v>1</v>
-      </c>
-      <c r="F10" s="129">
-        <v>1</v>
-      </c>
-      <c r="G10" s="129">
+      <c r="B10" s="124">
+        <v>1</v>
+      </c>
+      <c r="C10" s="125">
+        <v>1</v>
+      </c>
+      <c r="D10" s="125">
+        <v>1</v>
+      </c>
+      <c r="E10" s="125">
+        <v>1</v>
+      </c>
+      <c r="F10" s="125">
+        <v>1</v>
+      </c>
+      <c r="G10" s="125">
         <v>1</v>
       </c>
       <c r="H10" s="4">
@@ -2513,18 +2513,18 @@
       <c r="A11" s="75">
         <v>9</v>
       </c>
-      <c r="B11" s="130">
-        <v>1</v>
-      </c>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131">
-        <v>1</v>
-      </c>
-      <c r="F11" s="131">
-        <v>1</v>
-      </c>
-      <c r="G11" s="131">
+      <c r="B11" s="126">
+        <v>1</v>
+      </c>
+      <c r="C11" s="127"/>
+      <c r="D11" s="127"/>
+      <c r="E11" s="127">
+        <v>1</v>
+      </c>
+      <c r="F11" s="127">
+        <v>1</v>
+      </c>
+      <c r="G11" s="127">
         <v>1</v>
       </c>
       <c r="H11" s="5">
@@ -2539,27 +2539,27 @@
         <v>9</v>
       </c>
       <c r="C12" s="75">
-        <f>SUM(C2:C11)</f>
+        <f t="shared" ref="C12:H12" si="1">SUM(C2:C11)</f>
         <v>6</v>
       </c>
       <c r="D12" s="75">
-        <f>SUM(D2:D11)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="E12" s="75">
-        <f>SUM(E2:E11)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F12" s="75">
-        <f>SUM(F2:F11)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G12" s="75">
-        <f>SUM(G2:G11)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="H12" s="75">
-        <f>SUM(H2:H11)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I12" s="75"/>
@@ -2610,10 +2610,10 @@
       <c r="C9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="79" t="s">
+      <c r="D9" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="79"/>
+      <c r="E9" s="130"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -2650,10 +2650,10 @@
       <c r="C13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="79"/>
+      <c r="E13" s="130"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -2662,10 +2662,10 @@
       <c r="C14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="79" t="s">
+      <c r="D14" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="79"/>
+      <c r="E14" s="130"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -3878,16 +3878,16 @@
         <f>TRIM(_xlfn.CONCAT(IF(ISBLANK(D2),"",$D$1), " ", IF(ISBLANK(E2),"",$E$1), " ", IF(ISBLANK(F2),"",$F$1), " ", IF(ISBLANK(G2),"",$G$1), " ", IF(ISBLANK(H2),"",$H$1), " ", IF(ISBLANK(I2),"",$I$1), " ", IF(ISBLANK(J2),"",$J$1), " ", IF(ISBLANK(K2),"",$K$1), " ", IF(ISBLANK(L2),"",$L$1)))</f>
         <v>0 2</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="Q2" s="131" t="s">
         <v>77</v>
       </c>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81" t="s">
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="132" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
+      <c r="U2" s="132"/>
+      <c r="V2" s="132"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
@@ -4842,16 +4842,16 @@
         <f>TRIM(_xlfn.CONCAT(IF(ISBLANK(D2),"",$D$1), " ", IF(ISBLANK(E2),"",$E$1), " ", IF(ISBLANK(F2),"",$F$1), " ", IF(ISBLANK(G2),"",$G$1), " ", IF(ISBLANK(H2),"",$H$1), " ", IF(ISBLANK(I2),"",$I$1), " ", IF(ISBLANK(J2),"",$J$1), " ", IF(ISBLANK(K2),"",$K$1), " ", IF(ISBLANK(L2),"",$L$1)))</f>
         <v>0 2</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="Q2" s="131" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81" t="s">
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="132" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
+      <c r="U2" s="132"/>
+      <c r="V2" s="132"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
@@ -5331,16 +5331,16 @@
         <f>TRIM(_xlfn.CONCAT(IF(ISBLANK(D2),"",$D$1), " ", IF(ISBLANK(E2),"",$E$1), " ", IF(ISBLANK(F2),"",$F$1), " ", IF(ISBLANK(G2),"",$G$1), " ", IF(ISBLANK(H2),"",$H$1), " ", IF(ISBLANK(I2),"",$I$1), " ", IF(ISBLANK(J2),"",$J$1), " ", IF(ISBLANK(K2),"",$K$1), " ", IF(ISBLANK(L2),"",$L$1)))</f>
         <v>1 3</v>
       </c>
-      <c r="Q2" s="80" t="s">
+      <c r="Q2" s="131" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="81" t="s">
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
+      <c r="U2" s="132"/>
+      <c r="V2" s="132"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
@@ -5722,16 +5722,20 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.125" customWidth="1"/>
+    <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="3.5" customWidth="1"/>
-    <col min="20" max="20" width="6.625" customWidth="1"/>
+    <col min="3" max="3" width="6.125" customWidth="1"/>
+    <col min="4" max="9" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -6474,58 +6478,58 @@
       <c r="A16">
         <v>4</v>
       </c>
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="83" t="s">
+      <c r="C16" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="84">
-        <v>0</v>
-      </c>
-      <c r="E16" s="85">
-        <v>0</v>
-      </c>
-      <c r="F16" s="85">
-        <v>0</v>
-      </c>
-      <c r="G16" s="86">
-        <v>1</v>
-      </c>
-      <c r="H16" s="86">
-        <v>1</v>
-      </c>
-      <c r="I16" s="87">
-        <v>0</v>
-      </c>
-      <c r="J16" s="87">
-        <v>0</v>
-      </c>
-      <c r="K16" s="87">
-        <v>0</v>
-      </c>
-      <c r="L16" s="122">
-        <v>1</v>
-      </c>
-      <c r="M16" s="122">
-        <v>0</v>
-      </c>
-      <c r="N16" s="122">
-        <v>0</v>
-      </c>
-      <c r="O16" s="123">
-        <v>1</v>
-      </c>
-      <c r="P16" s="123">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="123">
-        <v>1</v>
-      </c>
-      <c r="R16" s="85">
-        <v>0</v>
-      </c>
-      <c r="S16" s="124">
+      <c r="D16" s="80">
+        <v>0</v>
+      </c>
+      <c r="E16" s="81">
+        <v>0</v>
+      </c>
+      <c r="F16" s="81">
+        <v>0</v>
+      </c>
+      <c r="G16" s="82">
+        <v>1</v>
+      </c>
+      <c r="H16" s="82">
+        <v>1</v>
+      </c>
+      <c r="I16" s="83">
+        <v>0</v>
+      </c>
+      <c r="J16" s="83">
+        <v>0</v>
+      </c>
+      <c r="K16" s="83">
+        <v>0</v>
+      </c>
+      <c r="L16" s="118">
+        <v>1</v>
+      </c>
+      <c r="M16" s="118">
+        <v>0</v>
+      </c>
+      <c r="N16" s="118">
+        <v>0</v>
+      </c>
+      <c r="O16" s="119">
+        <v>1</v>
+      </c>
+      <c r="P16" s="119">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="119">
+        <v>1</v>
+      </c>
+      <c r="R16" s="81">
+        <v>0</v>
+      </c>
+      <c r="S16" s="120">
         <v>0</v>
       </c>
       <c r="T16" t="str">
@@ -6537,58 +6541,58 @@
       <c r="A17">
         <v>5</v>
       </c>
-      <c r="B17" s="117" t="s">
+      <c r="B17" s="113" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="107">
-        <v>0</v>
-      </c>
-      <c r="E17" s="108">
-        <v>0</v>
-      </c>
-      <c r="F17" s="108">
-        <v>0</v>
-      </c>
-      <c r="G17" s="109">
-        <v>1</v>
-      </c>
-      <c r="H17" s="109">
-        <v>1</v>
-      </c>
-      <c r="I17" s="110">
-        <v>0</v>
-      </c>
-      <c r="J17" s="110">
-        <v>0</v>
-      </c>
-      <c r="K17" s="110">
-        <v>0</v>
-      </c>
-      <c r="L17" s="121">
-        <v>1</v>
-      </c>
-      <c r="M17" s="121">
-        <v>0</v>
-      </c>
-      <c r="N17" s="121">
-        <v>1</v>
-      </c>
-      <c r="O17" s="120">
-        <v>1</v>
-      </c>
-      <c r="P17" s="120">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="120">
-        <v>1</v>
-      </c>
-      <c r="R17" s="108">
-        <v>0</v>
-      </c>
-      <c r="S17" s="125">
+      <c r="D17" s="103">
+        <v>0</v>
+      </c>
+      <c r="E17" s="104">
+        <v>0</v>
+      </c>
+      <c r="F17" s="104">
+        <v>0</v>
+      </c>
+      <c r="G17" s="105">
+        <v>1</v>
+      </c>
+      <c r="H17" s="105">
+        <v>1</v>
+      </c>
+      <c r="I17" s="106">
+        <v>0</v>
+      </c>
+      <c r="J17" s="106">
+        <v>0</v>
+      </c>
+      <c r="K17" s="106">
+        <v>0</v>
+      </c>
+      <c r="L17" s="117">
+        <v>1</v>
+      </c>
+      <c r="M17" s="117">
+        <v>0</v>
+      </c>
+      <c r="N17" s="117">
+        <v>1</v>
+      </c>
+      <c r="O17" s="116">
+        <v>1</v>
+      </c>
+      <c r="P17" s="116">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="116">
+        <v>1</v>
+      </c>
+      <c r="R17" s="104">
+        <v>0</v>
+      </c>
+      <c r="S17" s="121">
         <v>0</v>
       </c>
       <c r="T17" t="str">
@@ -6600,58 +6604,58 @@
       <c r="A18">
         <v>6</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="84" t="s">
         <v>124</v>
       </c>
-      <c r="C18" s="89" t="s">
+      <c r="C18" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="D18" s="90">
-        <v>1</v>
-      </c>
-      <c r="E18" s="91">
-        <v>0</v>
-      </c>
-      <c r="F18" s="91">
-        <v>0</v>
-      </c>
-      <c r="G18" s="91">
-        <v>1</v>
-      </c>
-      <c r="H18" s="91">
-        <v>1</v>
-      </c>
-      <c r="I18" s="92">
-        <v>0</v>
-      </c>
-      <c r="J18" s="92">
-        <v>0</v>
-      </c>
-      <c r="K18" s="92">
-        <v>1</v>
-      </c>
-      <c r="L18" s="93">
-        <v>1</v>
-      </c>
-      <c r="M18" s="93">
-        <v>1</v>
-      </c>
-      <c r="N18" s="93">
-        <v>0</v>
-      </c>
-      <c r="O18" s="94">
-        <v>0</v>
-      </c>
-      <c r="P18" s="94">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="94">
-        <v>1</v>
-      </c>
-      <c r="R18" s="95">
-        <v>0</v>
-      </c>
-      <c r="S18" s="96">
+      <c r="D18" s="86">
+        <v>1</v>
+      </c>
+      <c r="E18" s="87">
+        <v>0</v>
+      </c>
+      <c r="F18" s="87">
+        <v>0</v>
+      </c>
+      <c r="G18" s="87">
+        <v>1</v>
+      </c>
+      <c r="H18" s="87">
+        <v>1</v>
+      </c>
+      <c r="I18" s="88">
+        <v>0</v>
+      </c>
+      <c r="J18" s="88">
+        <v>0</v>
+      </c>
+      <c r="K18" s="88">
+        <v>1</v>
+      </c>
+      <c r="L18" s="89">
+        <v>1</v>
+      </c>
+      <c r="M18" s="89">
+        <v>1</v>
+      </c>
+      <c r="N18" s="89">
+        <v>0</v>
+      </c>
+      <c r="O18" s="90">
+        <v>0</v>
+      </c>
+      <c r="P18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="90">
+        <v>1</v>
+      </c>
+      <c r="R18" s="91">
+        <v>0</v>
+      </c>
+      <c r="S18" s="92">
         <v>0</v>
       </c>
       <c r="T18" t="str">
@@ -6663,56 +6667,56 @@
       <c r="A19">
         <v>7</v>
       </c>
-      <c r="B19" s="88" t="s">
+      <c r="B19" s="84" t="s">
         <v>129</v>
       </c>
-      <c r="C19" s="89"/>
-      <c r="D19" s="90">
-        <v>1</v>
-      </c>
-      <c r="E19" s="91">
-        <v>0</v>
-      </c>
-      <c r="F19" s="91">
-        <v>1</v>
-      </c>
-      <c r="G19" s="91">
-        <v>1</v>
-      </c>
-      <c r="H19" s="91">
-        <v>1</v>
-      </c>
-      <c r="I19" s="92">
-        <v>0</v>
-      </c>
-      <c r="J19" s="92">
-        <v>1</v>
-      </c>
-      <c r="K19" s="92">
-        <v>1</v>
-      </c>
-      <c r="L19" s="93">
-        <v>0</v>
-      </c>
-      <c r="M19" s="93">
-        <v>0</v>
-      </c>
-      <c r="N19" s="93">
-        <v>1</v>
-      </c>
-      <c r="O19" s="94">
-        <v>1</v>
-      </c>
-      <c r="P19" s="94">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="94">
-        <v>1</v>
-      </c>
-      <c r="R19" s="95">
-        <v>0</v>
-      </c>
-      <c r="S19" s="96">
+      <c r="C19" s="85"/>
+      <c r="D19" s="86">
+        <v>1</v>
+      </c>
+      <c r="E19" s="87">
+        <v>0</v>
+      </c>
+      <c r="F19" s="87">
+        <v>1</v>
+      </c>
+      <c r="G19" s="87">
+        <v>1</v>
+      </c>
+      <c r="H19" s="87">
+        <v>1</v>
+      </c>
+      <c r="I19" s="88">
+        <v>0</v>
+      </c>
+      <c r="J19" s="88">
+        <v>1</v>
+      </c>
+      <c r="K19" s="88">
+        <v>1</v>
+      </c>
+      <c r="L19" s="89">
+        <v>0</v>
+      </c>
+      <c r="M19" s="89">
+        <v>0</v>
+      </c>
+      <c r="N19" s="89">
+        <v>1</v>
+      </c>
+      <c r="O19" s="90">
+        <v>1</v>
+      </c>
+      <c r="P19" s="90">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="90">
+        <v>1</v>
+      </c>
+      <c r="R19" s="91">
+        <v>0</v>
+      </c>
+      <c r="S19" s="92">
         <v>0</v>
       </c>
       <c r="T19" t="str">
@@ -6724,58 +6728,58 @@
       <c r="A20">
         <v>8</v>
       </c>
-      <c r="B20" s="118" t="s">
+      <c r="B20" s="114" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="111" t="s">
+      <c r="C20" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="112">
-        <v>0</v>
-      </c>
-      <c r="E20" s="113">
-        <v>0</v>
-      </c>
-      <c r="F20" s="113">
-        <v>0</v>
-      </c>
-      <c r="G20" s="114">
-        <v>1</v>
-      </c>
-      <c r="H20" s="114">
-        <v>1</v>
-      </c>
-      <c r="I20" s="115">
-        <v>1</v>
-      </c>
-      <c r="J20" s="115">
-        <v>0</v>
-      </c>
-      <c r="K20" s="115">
-        <v>1</v>
-      </c>
-      <c r="L20" s="116">
-        <v>0</v>
-      </c>
-      <c r="M20" s="116">
-        <v>0</v>
-      </c>
-      <c r="N20" s="116">
-        <v>0</v>
-      </c>
-      <c r="O20" s="132">
-        <v>0</v>
-      </c>
-      <c r="P20" s="132">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="132">
-        <v>1</v>
-      </c>
-      <c r="R20" s="113">
-        <v>0</v>
-      </c>
-      <c r="S20" s="119">
+      <c r="D20" s="108">
+        <v>0</v>
+      </c>
+      <c r="E20" s="109">
+        <v>0</v>
+      </c>
+      <c r="F20" s="109">
+        <v>0</v>
+      </c>
+      <c r="G20" s="110">
+        <v>1</v>
+      </c>
+      <c r="H20" s="110">
+        <v>1</v>
+      </c>
+      <c r="I20" s="111">
+        <v>1</v>
+      </c>
+      <c r="J20" s="111">
+        <v>0</v>
+      </c>
+      <c r="K20" s="111">
+        <v>1</v>
+      </c>
+      <c r="L20" s="112">
+        <v>0</v>
+      </c>
+      <c r="M20" s="112">
+        <v>0</v>
+      </c>
+      <c r="N20" s="112">
+        <v>0</v>
+      </c>
+      <c r="O20" s="128">
+        <v>0</v>
+      </c>
+      <c r="P20" s="128">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="128">
+        <v>1</v>
+      </c>
+      <c r="R20" s="109">
+        <v>0</v>
+      </c>
+      <c r="S20" s="115">
         <v>0</v>
       </c>
       <c r="T20" t="str">
@@ -6787,58 +6791,58 @@
       <c r="A21">
         <v>9</v>
       </c>
-      <c r="B21" s="117" t="s">
+      <c r="B21" s="113" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="107">
-        <v>0</v>
-      </c>
-      <c r="E21" s="108">
-        <v>0</v>
-      </c>
-      <c r="F21" s="108">
-        <v>0</v>
-      </c>
-      <c r="G21" s="109">
-        <v>1</v>
-      </c>
-      <c r="H21" s="109">
-        <v>1</v>
-      </c>
-      <c r="I21" s="110">
-        <v>0</v>
-      </c>
-      <c r="J21" s="110">
-        <v>0</v>
-      </c>
-      <c r="K21" s="110">
-        <v>0</v>
-      </c>
-      <c r="L21" s="121">
-        <v>1</v>
-      </c>
-      <c r="M21" s="121">
-        <v>0</v>
-      </c>
-      <c r="N21" s="121">
-        <v>1</v>
-      </c>
-      <c r="O21" s="120">
-        <v>1</v>
-      </c>
-      <c r="P21" s="120">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="120">
-        <v>1</v>
-      </c>
-      <c r="R21" s="108">
-        <v>0</v>
-      </c>
-      <c r="S21" s="125">
+      <c r="D21" s="103">
+        <v>0</v>
+      </c>
+      <c r="E21" s="104">
+        <v>0</v>
+      </c>
+      <c r="F21" s="104">
+        <v>0</v>
+      </c>
+      <c r="G21" s="105">
+        <v>1</v>
+      </c>
+      <c r="H21" s="105">
+        <v>1</v>
+      </c>
+      <c r="I21" s="106">
+        <v>0</v>
+      </c>
+      <c r="J21" s="106">
+        <v>0</v>
+      </c>
+      <c r="K21" s="106">
+        <v>0</v>
+      </c>
+      <c r="L21" s="117">
+        <v>1</v>
+      </c>
+      <c r="M21" s="117">
+        <v>0</v>
+      </c>
+      <c r="N21" s="117">
+        <v>1</v>
+      </c>
+      <c r="O21" s="116">
+        <v>1</v>
+      </c>
+      <c r="P21" s="116">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="116">
+        <v>1</v>
+      </c>
+      <c r="R21" s="104">
+        <v>0</v>
+      </c>
+      <c r="S21" s="121">
         <v>0</v>
       </c>
       <c r="T21" t="str">
@@ -6850,58 +6854,58 @@
       <c r="A22">
         <v>10</v>
       </c>
-      <c r="B22" s="88" t="s">
+      <c r="B22" s="84" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="89" t="s">
+      <c r="C22" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="90">
-        <v>1</v>
-      </c>
-      <c r="E22" s="91">
-        <v>0</v>
-      </c>
-      <c r="F22" s="91">
-        <v>1</v>
-      </c>
-      <c r="G22" s="91">
-        <v>1</v>
-      </c>
-      <c r="H22" s="91">
-        <v>1</v>
-      </c>
-      <c r="I22" s="92">
-        <v>0</v>
-      </c>
-      <c r="J22" s="92">
-        <v>0</v>
-      </c>
-      <c r="K22" s="92">
-        <v>1</v>
-      </c>
-      <c r="L22" s="93">
-        <v>1</v>
-      </c>
-      <c r="M22" s="93">
-        <v>1</v>
-      </c>
-      <c r="N22" s="93">
-        <v>0</v>
-      </c>
-      <c r="O22" s="94">
-        <v>0</v>
-      </c>
-      <c r="P22" s="94">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="94">
-        <v>1</v>
-      </c>
-      <c r="R22" s="95">
-        <v>0</v>
-      </c>
-      <c r="S22" s="96">
+      <c r="D22" s="86">
+        <v>1</v>
+      </c>
+      <c r="E22" s="87">
+        <v>0</v>
+      </c>
+      <c r="F22" s="87">
+        <v>1</v>
+      </c>
+      <c r="G22" s="87">
+        <v>1</v>
+      </c>
+      <c r="H22" s="87">
+        <v>1</v>
+      </c>
+      <c r="I22" s="88">
+        <v>0</v>
+      </c>
+      <c r="J22" s="88">
+        <v>0</v>
+      </c>
+      <c r="K22" s="88">
+        <v>1</v>
+      </c>
+      <c r="L22" s="89">
+        <v>1</v>
+      </c>
+      <c r="M22" s="89">
+        <v>1</v>
+      </c>
+      <c r="N22" s="89">
+        <v>0</v>
+      </c>
+      <c r="O22" s="90">
+        <v>0</v>
+      </c>
+      <c r="P22" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="90">
+        <v>1</v>
+      </c>
+      <c r="R22" s="91">
+        <v>0</v>
+      </c>
+      <c r="S22" s="92">
         <v>0</v>
       </c>
       <c r="T22" t="str">
@@ -6913,119 +6917,119 @@
       <c r="A23">
         <v>11</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="89"/>
-      <c r="D23" s="90">
-        <v>1</v>
-      </c>
-      <c r="E23" s="91">
-        <v>0</v>
-      </c>
-      <c r="F23" s="91">
-        <v>1</v>
-      </c>
-      <c r="G23" s="91">
-        <v>1</v>
-      </c>
-      <c r="H23" s="91">
-        <v>1</v>
-      </c>
-      <c r="I23" s="92">
-        <v>0</v>
-      </c>
-      <c r="J23" s="92">
-        <v>0</v>
-      </c>
-      <c r="K23" s="92">
-        <v>1</v>
-      </c>
-      <c r="L23" s="93">
-        <v>0</v>
-      </c>
-      <c r="M23" s="93">
-        <v>1</v>
-      </c>
-      <c r="N23" s="93">
-        <v>0</v>
-      </c>
-      <c r="O23" s="94">
-        <v>1</v>
-      </c>
-      <c r="P23" s="94">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="94">
-        <v>1</v>
-      </c>
-      <c r="R23" s="95">
-        <v>0</v>
-      </c>
-      <c r="S23" s="96">
+      <c r="C23" s="85"/>
+      <c r="D23" s="86">
+        <v>1</v>
+      </c>
+      <c r="E23" s="87">
+        <v>0</v>
+      </c>
+      <c r="F23" s="87">
+        <v>1</v>
+      </c>
+      <c r="G23" s="87">
+        <v>1</v>
+      </c>
+      <c r="H23" s="87">
+        <v>1</v>
+      </c>
+      <c r="I23" s="88">
+        <v>0</v>
+      </c>
+      <c r="J23" s="88">
+        <v>1</v>
+      </c>
+      <c r="K23" s="88">
+        <v>0</v>
+      </c>
+      <c r="L23" s="89">
+        <v>0</v>
+      </c>
+      <c r="M23" s="89">
+        <v>0</v>
+      </c>
+      <c r="N23" s="89">
+        <v>1</v>
+      </c>
+      <c r="O23" s="90">
+        <v>1</v>
+      </c>
+      <c r="P23" s="90">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="90">
+        <v>1</v>
+      </c>
+      <c r="R23" s="91">
+        <v>0</v>
+      </c>
+      <c r="S23" s="92">
         <v>0</v>
       </c>
       <c r="T23" t="str">
         <f t="shared" si="0"/>
-        <v>B95C</v>
+        <v>BA3C</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>12</v>
       </c>
-      <c r="B24" s="118" t="s">
+      <c r="B24" s="114" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="111" t="s">
+      <c r="C24" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="112">
-        <v>0</v>
-      </c>
-      <c r="E24" s="113">
-        <v>0</v>
-      </c>
-      <c r="F24" s="113">
-        <v>0</v>
-      </c>
-      <c r="G24" s="114">
-        <v>1</v>
-      </c>
-      <c r="H24" s="114">
-        <v>1</v>
-      </c>
-      <c r="I24" s="115">
-        <v>1</v>
-      </c>
-      <c r="J24" s="115">
-        <v>0</v>
-      </c>
-      <c r="K24" s="115">
-        <v>1</v>
-      </c>
-      <c r="L24" s="116">
-        <v>0</v>
-      </c>
-      <c r="M24" s="116">
-        <v>0</v>
-      </c>
-      <c r="N24" s="116">
-        <v>0</v>
-      </c>
-      <c r="O24" s="132">
-        <v>1</v>
-      </c>
-      <c r="P24" s="132">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="132">
-        <v>0</v>
-      </c>
-      <c r="R24" s="113">
-        <v>0</v>
-      </c>
-      <c r="S24" s="119">
+      <c r="D24" s="108">
+        <v>0</v>
+      </c>
+      <c r="E24" s="109">
+        <v>0</v>
+      </c>
+      <c r="F24" s="109">
+        <v>0</v>
+      </c>
+      <c r="G24" s="110">
+        <v>1</v>
+      </c>
+      <c r="H24" s="110">
+        <v>1</v>
+      </c>
+      <c r="I24" s="111">
+        <v>1</v>
+      </c>
+      <c r="J24" s="111">
+        <v>0</v>
+      </c>
+      <c r="K24" s="111">
+        <v>1</v>
+      </c>
+      <c r="L24" s="112">
+        <v>0</v>
+      </c>
+      <c r="M24" s="112">
+        <v>0</v>
+      </c>
+      <c r="N24" s="112">
+        <v>0</v>
+      </c>
+      <c r="O24" s="128">
+        <v>1</v>
+      </c>
+      <c r="P24" s="128">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="128">
+        <v>0</v>
+      </c>
+      <c r="R24" s="109">
+        <v>0</v>
+      </c>
+      <c r="S24" s="115">
         <v>0</v>
       </c>
       <c r="T24" t="str">
@@ -7037,63 +7041,63 @@
       <c r="A25">
         <v>13</v>
       </c>
-      <c r="B25" s="97" t="s">
+      <c r="B25" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="C25" s="98" t="s">
+      <c r="C25" s="94" t="s">
         <v>121</v>
       </c>
-      <c r="D25" s="99">
-        <v>0</v>
-      </c>
-      <c r="E25" s="100">
-        <v>0</v>
-      </c>
-      <c r="F25" s="100">
-        <v>0</v>
-      </c>
-      <c r="G25" s="101">
-        <v>1</v>
-      </c>
-      <c r="H25" s="101">
-        <v>1</v>
-      </c>
-      <c r="I25" s="102">
-        <v>1</v>
-      </c>
-      <c r="J25" s="102">
-        <v>0</v>
-      </c>
-      <c r="K25" s="102">
-        <v>1</v>
-      </c>
-      <c r="L25" s="103">
-        <v>0</v>
-      </c>
-      <c r="M25" s="103">
-        <v>0</v>
-      </c>
-      <c r="N25" s="103">
-        <v>0</v>
-      </c>
-      <c r="O25" s="104">
-        <v>1</v>
-      </c>
-      <c r="P25" s="104">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="104">
-        <v>1</v>
-      </c>
-      <c r="R25" s="100">
-        <v>0</v>
-      </c>
-      <c r="S25" s="105">
+      <c r="D25" s="95">
+        <v>0</v>
+      </c>
+      <c r="E25" s="96">
+        <v>0</v>
+      </c>
+      <c r="F25" s="96">
+        <v>0</v>
+      </c>
+      <c r="G25" s="97">
+        <v>1</v>
+      </c>
+      <c r="H25" s="97">
+        <v>1</v>
+      </c>
+      <c r="I25" s="98">
+        <v>1</v>
+      </c>
+      <c r="J25" s="98">
+        <v>0</v>
+      </c>
+      <c r="K25" s="98">
+        <v>0</v>
+      </c>
+      <c r="L25" s="99">
+        <v>0</v>
+      </c>
+      <c r="M25" s="99">
+        <v>0</v>
+      </c>
+      <c r="N25" s="99">
+        <v>0</v>
+      </c>
+      <c r="O25" s="100">
+        <v>1</v>
+      </c>
+      <c r="P25" s="100">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="100">
+        <v>1</v>
+      </c>
+      <c r="R25" s="96">
+        <v>0</v>
+      </c>
+      <c r="S25" s="101">
         <v>0</v>
       </c>
       <c r="T25" t="str">
         <f t="shared" si="0"/>
-        <v>1D1C</v>
+        <v>1C1C</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>